<commit_message>
fixed a few bugs
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prave\Desktop\tech-projects\medium-projects\telegram-bot\AngelMortalTelegraf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C396119-36E6-4E5A-938C-EC2DE3B29480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7301AF6D-24D9-4AAE-BB25-32EDEBE0AA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Mortal</t>
   </si>
@@ -36,15 +36,6 @@
     <t>joanne</t>
   </si>
   <si>
-    <t>nick</t>
-  </si>
-  <si>
-    <t>casper</t>
-  </si>
-  <si>
-    <t>daniel</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -141,19 +132,34 @@
     <t>lol</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>2l</t>
-  </si>
-  <si>
-    <t>3l</t>
-  </si>
-  <si>
-    <t>4l</t>
-  </si>
-  <si>
-    <t>5l</t>
+    <t>chelsea</t>
+  </si>
+  <si>
+    <t>dayna</t>
+  </si>
+  <si>
+    <t>kelsy</t>
+  </si>
+  <si>
+    <t>personA</t>
+  </si>
+  <si>
+    <t>personB</t>
+  </si>
+  <si>
+    <t>personC</t>
+  </si>
+  <si>
+    <t>lol2</t>
+  </si>
+  <si>
+    <t>lol3</t>
+  </si>
+  <si>
+    <t>lol4</t>
+  </si>
+  <si>
+    <t>lol5</t>
   </si>
 </sst>
 </file>
@@ -471,150 +477,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>31</v>
-      </c>
-      <c r="G6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -622,22 +628,68 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B8" t="s">
         <v>39</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>42</v>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>